<commit_message>
work on paper regression and stuff
</commit_message>
<xml_diff>
--- a/regression.xlsx
+++ b/regression.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moe\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\SpeedNeverKilledSomebody\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA9638E-7851-402F-BD2A-1B0A1B299DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7873E038-06B3-412F-BEBD-974200CA7A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E98E9116-AD71-44A5-9371-F68D31F0AF7A}"/>
+    <workbookView xWindow="3612" yWindow="17172" windowWidth="23256" windowHeight="12720" xr2:uid="{E98E9116-AD71-44A5-9371-F68D31F0AF7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Disp</t>
+  </si>
+  <si>
+    <t>1/Disp</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -98,12 +112,37 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Disparity Depth Relation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.8600174978129328E-4"/>
-          <c:y val="0"/>
+          <c:x val="0.32718377073406091"/>
+          <c:y val="4.6296313173050878E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -119,11 +158,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -131,95 +170,187 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11824490338299963"/>
+          <c:y val="0.19226858860768031"/>
+          <c:w val="0.83907755669175399"/>
+          <c:h val="0.61706788315393812"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400">
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.68988715277778001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56168619791666996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43098958333332998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.41389973958332998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.36149088541667002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31993272569443998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.28879123263889001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25922309027778001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23491753472221999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.21847873263889001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.20421006944444001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-2771-4F0F-99A8-E807DEB7BBA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
+              <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="4"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.15322619838760565"/>
-                  <c:y val="0.11987617600414838"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-DE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$A$1:$A$11</c:f>
+              <c:f>Tabelle1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -261,7 +392,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$B$11</c:f>
+              <c:f>Tabelle1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -304,7 +435,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-089D-40EE-AF91-6F6836D81B30}"/>
+              <c16:uniqueId val="{00000004-2771-4F0F-99A8-E807DEB7BBA9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -330,7 +461,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -340,20 +471,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Depth</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -364,9 +544,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -374,7 +554,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1436513440"/>
@@ -392,7 +572,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -402,20 +582,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Disparity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -426,9 +655,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -436,7 +665,675 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1436523008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="43000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Inverse Disparity - Depth Relation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13640472866666012"/>
+          <c:y val="3.6717877937671582E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11824490338299963"/>
+          <c:y val="0.19226858860768031"/>
+          <c:w val="0.83907755669175399"/>
+          <c:h val="0.61706788315393812"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.4495124252909672</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7803535207186219</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3202416918429183</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4160440424695437</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7663214768122213</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1256571137867146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4627089986849389</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8576810380912185</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.2568129330254445</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5771045443257776</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.8969181721573856</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-06DA-432F-BA45-7443578B9267}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1436523008"/>
+        <c:axId val="1436513440"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:ln w="25400">
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="4"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:trendline>
+                  <c:spPr>
+                    <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1">
+                          <a:alpha val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:trendlineType val="poly"/>
+                  <c:order val="4"/>
+                  <c:dispRSqr val="0"/>
+                  <c:dispEq val="0"/>
+                </c:trendline>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$A$2:$A$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>80</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>110</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>120</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>130</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>140</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>150</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$B$2:$B$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>0.68988715277778001</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.56168619791666996</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.43098958333332998</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.41389973958332998</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.36149088541667002</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.31993272569443998</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.28879123263889001</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.25922309027778001</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.23491753472221999</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.21847873263889001</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.20421006944444001</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-06DA-432F-BA45-7443578B9267}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1436523008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Inverse Depth</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1436513440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1436513440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Disparity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1436523008"/>
@@ -463,12 +1360,25 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="43000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -484,7 +1394,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DE"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -535,36 +1445,76 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="244">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -572,20 +1522,33 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="43000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -593,16 +1556,16 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -619,16 +1582,11 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -637,39 +1595,50 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="20000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
@@ -677,7 +1646,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -685,14 +1654,18 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -700,7 +1673,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -716,16 +1689,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -749,14 +1721,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -768,14 +1739,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -787,14 +1757,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -805,12 +1774,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -822,7 +1785,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -841,7 +1804,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
@@ -858,49 +1821,567 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" kern="1200" spc="70" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="244">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="43000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="20000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -908,7 +2389,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -922,10 +2403,20 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -936,14 +2427,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -952,16 +2442,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="0" kern="1200" spc="70" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
+      <cs:styleClr val="0"/>
     </cs:lnRef>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -969,11 +2459,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
+      <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -982,9 +2474,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1000,14 +2492,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1016,22 +2507,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1041,12 +2521,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1055,16 +2529,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>641985</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>185736</xdr:rowOff>
+      <xdr:rowOff>83821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1084,6 +2558,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>53339</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA7641A7-3116-4D12-9596-C2D56974A424}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1389,100 +2901,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6B435F-3318-4D4C-B507-A3F432B421DD}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>50</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>0.68988715277778001</v>
       </c>
+      <c r="C2">
+        <f>1/B2</f>
+        <v>1.4495124252909672</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>60</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>0.56168619791666996</v>
       </c>
+      <c r="C3">
+        <f>1/B3</f>
+        <v>1.7803535207186219</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>70</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>0.43098958333332998</v>
       </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C12" si="0">1/B4</f>
+        <v>2.3202416918429183</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>80</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>0.41389973958332998</v>
       </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>2.4160440424695437</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>90</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>0.36149088541667002</v>
       </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>2.7663214768122213</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>100</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>0.31993272569443998</v>
       </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>3.1256571137867146</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>110</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>0.28879123263889001</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>3.4627089986849389</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>120</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>0.25922309027778001</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>3.8576810380912185</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>130</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>0.23491753472221999</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>4.2568129330254445</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>140</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>0.21847873263889001</v>
       </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>4.5771045443257776</v>
+      </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>150</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>0.20421006944444001</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>4.8969181721573856</v>
       </c>
     </row>
   </sheetData>

</xml_diff>